<commit_message>
Add tilt angle of PS10.
</commit_message>
<xml_diff>
--- a/PS10/parameters.xlsx
+++ b/PS10/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sth\Desktop\2022年光热太阳能仿真与建模\太阳能镜场数据整理\PS10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6B480-F085-44DE-9E58-C2DFE2CBC634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90F0711-A02F-4D2C-B2B1-51B41D328438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
   <si>
     <t>位置</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -393,6 +393,25 @@
   </si>
   <si>
     <t>width per panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.5 °</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tilt angle</t>
+  </si>
+  <si>
+    <t>接收器倾斜角度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[3]. Belaid A, Filali A, Hassani S, et al. Heliostat field optimization and comparisons between biomimetic spiral and radial-staggered layouts for different heliostat shapes[J]. Solar Energy, 2022, 238: 162-177.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,6 +485,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -753,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -777,7 +799,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -786,42 +808,42 @@
       <c r="C2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -830,30 +852,30 @@
       <c r="C6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3">
         <v>0.05</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -862,110 +884,110 @@
       <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>624</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="3">
         <v>0.88</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -974,66 +996,83 @@
       <c r="C20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C22" s="3">
         <v>4</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>79</v>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1041,8 +1080,8 @@
     <mergeCell ref="A9:A19"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A20:A25"/>
     <mergeCell ref="D2:D25"/>
+    <mergeCell ref="A20:A26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1052,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E56D1C-CF4D-4FCA-A2A0-34606D159E38}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1077,7 +1116,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1086,50 +1125,50 @@
       <c r="C2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>80</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1138,36 +1177,36 @@
       <c r="C6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="1">
         <v>0.05</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1176,132 +1215,132 @@
       <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="1">
         <v>624</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="3">
         <v>0.88</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1310,84 +1349,103 @@
       <c r="C20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1395,8 +1453,8 @@
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A19"/>
-    <mergeCell ref="A20:A25"/>
     <mergeCell ref="D2:D25"/>
+    <mergeCell ref="A20:A26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>